<commit_message>
Actualización SmartScore desde Streamlit (Juan)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -614,10 +614,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0.548</t>
-        </is>
+      <c r="E2" t="n">
+        <v>0.548</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -629,10 +627,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0.489</t>
-        </is>
+      <c r="H2" t="n">
+        <v>0.489</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -644,10 +640,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>0.477</t>
-        </is>
+      <c r="K2" t="n">
+        <v>0.477</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -659,10 +653,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>0.605</t>
-        </is>
+      <c r="N2" t="n">
+        <v>0.605</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -674,10 +666,8 @@
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>0.602</t>
-        </is>
+      <c r="Q2" t="n">
+        <v>0.602</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
@@ -689,10 +679,8 @@
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>0.555</t>
-        </is>
+      <c r="T2" t="n">
+        <v>0.555</v>
       </c>
       <c r="U2" t="inlineStr">
         <is>
@@ -704,10 +692,8 @@
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>0.719</t>
-        </is>
+      <c r="W2" t="n">
+        <v>0.719</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
@@ -719,27 +705,183 @@
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="Z2" t="n">
+        <v>0.601</v>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.576</v>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-10-28 02:50:18</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.4,
+  "diet": 0.8571428571428571,
+  "salt": 0.6,
+  "fat": 1.0,
+  "natural": 0.8,
+  "convenience": 0.2,
+  "price": 0.8
+}</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.533</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.475</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.426</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>0.703</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>0.639</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>0.552</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>0.698</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
         <is>
           <t>0.601</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AA3" t="inlineStr">
         <is>
           <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AB3" t="inlineStr">
         <is>
           <t>Jack Link’s Beef Jerky Original</t>
         </is>
       </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>0.576</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>0.579</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
         <is>
           <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
         </is>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Salvador Vidal)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -584,6 +584,21 @@
           <t>Ready to Eat · Top 3 · Comentarios</t>
         </is>
       </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre Completo</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Edad</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Género</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -726,6 +741,9 @@
           <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
         </is>
       </c>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -756,10 +774,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0.533</t>
-        </is>
+      <c r="E3" t="n">
+        <v>0.533</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -771,10 +787,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0.475</t>
-        </is>
+      <c r="H3" t="n">
+        <v>0.475</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -786,10 +800,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0.426</t>
-        </is>
+      <c r="K3" t="n">
+        <v>0.426</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -801,10 +813,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>0.703</t>
-        </is>
+      <c r="N3" t="n">
+        <v>0.703</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -816,10 +826,8 @@
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>0.639</t>
-        </is>
+      <c r="Q3" t="n">
+        <v>0.639</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
@@ -831,10 +839,8 @@
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>0.552</t>
-        </is>
+      <c r="T3" t="n">
+        <v>0.552</v>
       </c>
       <c r="U3" t="inlineStr">
         <is>
@@ -846,10 +852,8 @@
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>0.698</t>
-        </is>
+      <c r="W3" t="n">
+        <v>0.698</v>
       </c>
       <c r="X3" t="inlineStr">
         <is>
@@ -861,10 +865,8 @@
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>0.601</t>
-        </is>
+      <c r="Z3" t="n">
+        <v>0.601</v>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
@@ -876,14 +878,188 @@
           <t>Jack Link’s Beef Jerky Original</t>
         </is>
       </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>0.579</t>
-        </is>
+      <c r="AC3" t="n">
+        <v>0.579</v>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
           <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Salvador Vidal</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-10-28 04:13:10</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 0.42857142857142855,
+  "salt": 0.4,
+  "fat": 0.8,
+  "natural": 0.8,
+  "convenience": 0.2,
+  "price": 0.6
+}</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.627</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.469</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0.458</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>0.696</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>0.640</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>0.577</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>0.679</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>0.545</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>0.516</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>Salvador Vidal</t>
+        </is>
+      </c>
+      <c r="AF4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>Masculino</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Juan Luis)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -632,10 +632,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0.627</t>
-        </is>
+      <c r="G2" t="n">
+        <v>0.627</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -647,10 +645,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0.469</t>
-        </is>
+      <c r="J2" t="n">
+        <v>0.469</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -662,10 +658,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>0.458</t>
-        </is>
+      <c r="M2" t="n">
+        <v>0.458</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -677,10 +671,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>0.696</t>
-        </is>
+      <c r="P2" t="n">
+        <v>0.696</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -692,10 +684,8 @@
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>0.640</t>
-        </is>
+      <c r="S2" t="n">
+        <v>0.64</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -707,10 +697,8 @@
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>0.577</t>
-        </is>
+      <c r="V2" t="n">
+        <v>0.577</v>
       </c>
       <c r="W2" t="inlineStr">
         <is>
@@ -722,10 +710,8 @@
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>0.679</t>
-        </is>
+      <c r="Y2" t="n">
+        <v>0.679</v>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
@@ -737,10 +723,8 @@
           <t>Kitchens of India Variety Pack</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>0.545</t>
-        </is>
+      <c r="AB2" t="n">
+        <v>0.545</v>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
@@ -752,12 +736,178 @@
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>0.516</t>
-        </is>
+      <c r="AE2" t="n">
+        <v>0.516</v>
       </c>
       <c r="AF2" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Juan Luis</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>24</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-10-28 05:27:34</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 1.0,
+  "salt": 0.8,
+  "fat": 0.0,
+  "natural": 0.8,
+  "convenience": 0.2,
+  "price": 0.2
+}</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.572</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.514</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0.409</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>0.845</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>0.618</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>0.602</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>0.769</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>0.503</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>0.423</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
         <is>
           <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
         </is>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Rosa Linda)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -782,134 +782,284 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" t="n">
+        <v>0.572</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>0.514</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>0.409</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>0.618</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="V3" t="n">
+        <v>0.602</v>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.769</v>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.503</v>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AE3" t="n">
+        <v>0.423</v>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Rosa Linda</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Femenino</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-10-28 05:43:11</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.4,
+  "diet": 0.7142857142857143,
+  "salt": 0.4,
+  "fat": 1.0,
+  "natural": 1.0,
+  "convenience": 0.8,
+  "price": 0.8
+}</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>0.572</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0.488</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>0.514</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>0.412</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
         <is>
           <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Nongshim Shin Ramyun</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>0.409</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>0.636</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>0.578</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
         <is>
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>0.845</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>0.541</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
         <is>
           <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Kraft Macaroni &amp; Cheese Dinner</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>0.618</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Annie’s Shells &amp; White Cheddar</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>0.602</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
+      <c r="X4" t="inlineStr">
         <is>
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>0.769</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>0.738</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
         <is>
           <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>Kitchens of India Variety Pack</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>0.503</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
+      <c r="AA4" t="inlineStr">
         <is>
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>0.423</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>0.614</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
         <is>
           <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>0.599</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Miranda)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -932,10 +932,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0.572</t>
-        </is>
+      <c r="G4" t="n">
+        <v>0.572</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -947,10 +945,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>0.488</t>
-        </is>
+      <c r="J4" t="n">
+        <v>0.488</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -962,10 +958,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>0.412</t>
-        </is>
+      <c r="M4" t="n">
+        <v>0.412</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -977,10 +971,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>0.636</t>
-        </is>
+      <c r="P4" t="n">
+        <v>0.636</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -992,10 +984,8 @@
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>0.578</t>
-        </is>
+      <c r="S4" t="n">
+        <v>0.578</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
@@ -1007,10 +997,8 @@
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>0.541</t>
-        </is>
+      <c r="V4" t="n">
+        <v>0.541</v>
       </c>
       <c r="W4" t="inlineStr">
         <is>
@@ -1022,10 +1010,8 @@
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>0.738</t>
-        </is>
+      <c r="Y4" t="n">
+        <v>0.738</v>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
@@ -1037,10 +1023,8 @@
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>0.614</t>
-        </is>
+      <c r="AB4" t="n">
+        <v>0.614</v>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
@@ -1052,12 +1036,178 @@
           <t>Jack Link’s Beef Jerky Original</t>
         </is>
       </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>0.599</t>
-        </is>
+      <c r="AE4" t="n">
+        <v>0.599</v>
       </c>
       <c r="AF4" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Miranda</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>25</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Femenino</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-10-28 05:51:45</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 0.5714285714285714,
+  "salt": 0.6,
+  "fat": 0.8,
+  "natural": 0.6,
+  "convenience": 0.4,
+  "price": 0.8
+}</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.575</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0.510</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>0.509</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>0.650</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>0.587</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>0.552</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>0.664</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>0.589</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>0.576</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
         <is>
           <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
         </is>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Joselyn)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF8"/>
+  <dimension ref="A1:AF9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1532,10 +1532,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>0.575</t>
-        </is>
+      <c r="G8" t="n">
+        <v>0.575</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1547,10 +1545,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>0.510</t>
-        </is>
+      <c r="J8" t="n">
+        <v>0.51</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -1562,10 +1558,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>0.509</t>
-        </is>
+      <c r="M8" t="n">
+        <v>0.509</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -1577,10 +1571,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>0.650</t>
-        </is>
+      <c r="P8" t="n">
+        <v>0.65</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -1592,10 +1584,8 @@
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>0.587</t>
-        </is>
+      <c r="S8" t="n">
+        <v>0.587</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
@@ -1607,10 +1597,8 @@
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>0.552</t>
-        </is>
+      <c r="V8" t="n">
+        <v>0.552</v>
       </c>
       <c r="W8" t="inlineStr">
         <is>
@@ -1622,10 +1610,8 @@
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>0.664</t>
-        </is>
+      <c r="Y8" t="n">
+        <v>0.664</v>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
@@ -1637,10 +1623,8 @@
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>0.589</t>
-        </is>
+      <c r="AB8" t="n">
+        <v>0.589</v>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
@@ -1652,14 +1636,180 @@
           <t>Jack Link’s Beef Jerky Original</t>
         </is>
       </c>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>0.576</t>
-        </is>
+      <c r="AE8" t="n">
+        <v>0.576</v>
       </c>
       <c r="AF8" t="inlineStr">
         <is>
           <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Joselyn</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>26</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Femenino</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-10-28 06:05:38</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 0.2857142857142857,
+  "salt": 0.8,
+  "fat": 1.0,
+  "natural": 0.8,
+  "convenience": 0.2,
+  "price": 0.4
+}</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.568</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0.483</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>0.447</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>0.731</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>0.690</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>0.582</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>0.704</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>0.611</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>0.573</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (serie lote)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF9"/>
+  <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1682,10 +1682,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>0.568</t>
-        </is>
+      <c r="G9" t="n">
+        <v>0.5679999999999999</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1697,10 +1695,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>0.483</t>
-        </is>
+      <c r="J9" t="n">
+        <v>0.483</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -1712,10 +1708,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>0.447</t>
-        </is>
+      <c r="M9" t="n">
+        <v>0.447</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1727,10 +1721,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>0.731</t>
-        </is>
+      <c r="P9" t="n">
+        <v>0.731</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
@@ -1742,10 +1734,8 @@
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>0.690</t>
-        </is>
+      <c r="S9" t="n">
+        <v>0.6899999999999999</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
@@ -1757,10 +1747,8 @@
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>0.582</t>
-        </is>
+      <c r="V9" t="n">
+        <v>0.582</v>
       </c>
       <c r="W9" t="inlineStr">
         <is>
@@ -1772,10 +1760,8 @@
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>0.704</t>
-        </is>
+      <c r="Y9" t="n">
+        <v>0.704</v>
       </c>
       <c r="Z9" t="inlineStr">
         <is>
@@ -1787,10 +1773,8 @@
           <t>Kitchens of India Variety Pack</t>
         </is>
       </c>
-      <c r="AB9" t="inlineStr">
-        <is>
-          <t>0.611</t>
-        </is>
+      <c r="AB9" t="n">
+        <v>0.611</v>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
@@ -1802,14 +1786,180 @@
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="AE9" t="inlineStr">
-        <is>
-          <t>0.573</t>
-        </is>
+      <c r="AE9" t="n">
+        <v>0.573</v>
       </c>
       <c r="AF9" t="inlineStr">
         <is>
           <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>serie lote</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>32</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-10-28 06:12:03</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 0.2857142857142857,
+  "salt": 1.0,
+  "fat": 0.6,
+  "natural": 0.2,
+  "convenience": 0.8,
+  "price": 0.6
+}</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.592</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.574</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>0.506</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>0.636</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>0.581</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>0.549</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>0.703</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>0.699</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>0.675</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (jOSE)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF10"/>
+  <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1832,10 +1832,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0.592</t>
-        </is>
+      <c r="G10" t="n">
+        <v>0.592</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1847,10 +1845,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>0.574</t>
-        </is>
+      <c r="J10" t="n">
+        <v>0.574</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -1862,10 +1858,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>0.506</t>
-        </is>
+      <c r="M10" t="n">
+        <v>0.506</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1877,10 +1871,8 @@
           <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>0.636</t>
-        </is>
+      <c r="P10" t="n">
+        <v>0.636</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
@@ -1892,10 +1884,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>0.581</t>
-        </is>
+      <c r="S10" t="n">
+        <v>0.581</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
@@ -1907,10 +1897,8 @@
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>0.549</t>
-        </is>
+      <c r="V10" t="n">
+        <v>0.549</v>
       </c>
       <c r="W10" t="inlineStr">
         <is>
@@ -1922,10 +1910,8 @@
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>0.703</t>
-        </is>
+      <c r="Y10" t="n">
+        <v>0.703</v>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
@@ -1937,10 +1923,8 @@
           <t>Jack Link’s Beef Jerky Original</t>
         </is>
       </c>
-      <c r="AB10" t="inlineStr">
-        <is>
-          <t>0.699</t>
-        </is>
+      <c r="AB10" t="n">
+        <v>0.699</v>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
@@ -1952,14 +1936,180 @@
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="AE10" t="inlineStr">
-        <is>
-          <t>0.675</t>
-        </is>
+      <c r="AE10" t="n">
+        <v>0.675</v>
       </c>
       <c r="AF10" t="inlineStr">
         <is>
           <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>jOSE</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>23</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-10-31 00:47:48</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 0.2857142857142857,
+  "salt": 0.8,
+  "fat": 0.2,
+  "natural": 0.6,
+  "convenience": 0.4,
+  "price": 0.2
+}</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.588</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.538</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>0.433</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0.729</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>0.630</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>0.608</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>0.733</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>0.599</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>0.518</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Gerarado Juan)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -648,10 +648,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>0.620</t>
-        </is>
+      <c r="I2" t="n">
+        <v>0.62</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -663,10 +661,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>0.541</t>
-        </is>
+      <c r="L2" t="n">
+        <v>0.541</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -678,10 +674,8 @@
           <t>Nongshim Shin Ramyun</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>0.532</t>
-        </is>
+      <c r="O2" t="n">
+        <v>0.532</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -693,10 +687,8 @@
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>0.632</t>
-        </is>
+      <c r="R2" t="n">
+        <v>0.632</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
@@ -708,10 +700,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>0.597</t>
-        </is>
+      <c r="U2" t="n">
+        <v>0.597</v>
       </c>
       <c r="V2" t="inlineStr">
         <is>
@@ -723,10 +713,8 @@
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>0.554</t>
-        </is>
+      <c r="X2" t="n">
+        <v>0.554</v>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
@@ -738,10 +726,8 @@
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>0.678</t>
-        </is>
+      <c r="AA2" t="n">
+        <v>0.678</v>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
@@ -753,10 +739,8 @@
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>0.472</t>
-        </is>
+      <c r="AD2" t="n">
+        <v>0.472</v>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
@@ -768,14 +752,186 @@
           <t>Kitchens of India Variety Pack</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>0.441</t>
-        </is>
+      <c r="AG2" t="n">
+        <v>0.441</v>
       </c>
       <c r="AH2" t="inlineStr">
         <is>
           <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Gerarado Juan_20251113_181055</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Gerarado Juan</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>21</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-13 18:10:55</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.4,
+  "diet": 0.7142857142857143,
+  "salt": 0.4,
+  "fat": 0.8,
+  "natural": 0.8,
+  "convenience": 0.4,
+  "price": 0.6
+}</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0.563</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>0.454</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>0.418</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>0.663</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>0.608</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>0.576</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>0.730</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>0.580</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>0.556</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Julieta Hernandez)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -804,10 +804,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0.563</t>
-        </is>
+      <c r="I3" t="n">
+        <v>0.5629999999999999</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -819,10 +817,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>0.454</t>
-        </is>
+      <c r="L3" t="n">
+        <v>0.454</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -834,10 +830,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>0.418</t>
-        </is>
+      <c r="O3" t="n">
+        <v>0.418</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -849,10 +843,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>0.663</t>
-        </is>
+      <c r="R3" t="n">
+        <v>0.663</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
@@ -864,10 +856,8 @@
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>0.608</t>
-        </is>
+      <c r="U3" t="n">
+        <v>0.608</v>
       </c>
       <c r="V3" t="inlineStr">
         <is>
@@ -879,10 +869,8 @@
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>0.576</t>
-        </is>
+      <c r="X3" t="n">
+        <v>0.576</v>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
@@ -894,10 +882,8 @@
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>0.730</t>
-        </is>
+      <c r="AA3" t="n">
+        <v>0.73</v>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
@@ -909,10 +895,8 @@
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>0.580</t>
-        </is>
+      <c r="AD3" t="n">
+        <v>0.58</v>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
@@ -924,14 +908,186 @@
           <t>Jack Link’s Beef Jerky Original</t>
         </is>
       </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>0.556</t>
-        </is>
+      <c r="AG3" t="n">
+        <v>0.556</v>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
           <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Julieta Hernandez_20251113_204328</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Julieta Hernandez</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>22</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-11-13 20:43:29</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.6,
+  "diet": 0.14285714285714285,
+  "salt": 0.4,
+  "fat": 1.0,
+  "natural": 0.4,
+  "convenience": 0.6,
+  "price": 0.8
+}</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0.612</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>0.573</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>0.496</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>0.643</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>0.626</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>0.568</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>0.695</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>0.686</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>0.645</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Fernanda Adamaris)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH4"/>
+  <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -960,10 +960,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>0.612</t>
-        </is>
+      <c r="I4" t="n">
+        <v>0.612</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -975,10 +973,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>0.573</t>
-        </is>
+      <c r="L4" t="n">
+        <v>0.573</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -990,10 +986,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>0.496</t>
-        </is>
+      <c r="O4" t="n">
+        <v>0.496</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -1005,89 +999,251 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="R4" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="U4" t="n">
+        <v>0.626</v>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X4" t="n">
+        <v>0.5679999999999999</v>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AA4" t="n">
+        <v>0.695</v>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.6860000000000001</v>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AG4" t="n">
+        <v>0.645</v>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Fernanda Adamaris_20251113_204405</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Fernanda Adamaris</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-11-13 20:44:06</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.4,
+  "diet": 0.14285714285714285,
+  "salt": 0.2,
+  "fat": 0.4,
+  "natural": 0.2,
+  "convenience": 0.2,
+  "price": 0.4
+}</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0.600</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0.563</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>0.539</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
         <is>
           <t>0.643</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>0.626</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>0.582</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
         <is>
           <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
+      <c r="W5" t="inlineStr">
         <is>
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>0.568</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>0.569</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
         <is>
           <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
         </is>
       </c>
-      <c r="Z4" t="inlineStr">
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>0.624</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>0.611</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
         <is>
           <t>Jack Link’s Beef Jerky Original</t>
         </is>
       </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>0.695</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>0.611</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
         <is>
           <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>StarKist Chicken Creations (Chicken Salad)</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>0.686</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>Wild Planet Wild Tuna Pasta Salad</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>0.645</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Hanna Moriel)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH5"/>
+  <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1116,10 +1116,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>0.600</t>
-        </is>
+      <c r="I5" t="n">
+        <v>0.6</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -1131,10 +1129,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>0.563</t>
-        </is>
+      <c r="L5" t="n">
+        <v>0.5629999999999999</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -1146,10 +1142,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>0.539</t>
-        </is>
+      <c r="O5" t="n">
+        <v>0.539</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
@@ -1161,10 +1155,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>0.643</t>
-        </is>
+      <c r="R5" t="n">
+        <v>0.643</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
@@ -1176,10 +1168,8 @@
           <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>0.582</t>
-        </is>
+      <c r="U5" t="n">
+        <v>0.582</v>
       </c>
       <c r="V5" t="inlineStr">
         <is>
@@ -1191,10 +1181,8 @@
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>0.569</t>
-        </is>
+      <c r="X5" t="n">
+        <v>0.569</v>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
@@ -1206,10 +1194,8 @@
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>0.624</t>
-        </is>
+      <c r="AA5" t="n">
+        <v>0.624</v>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
@@ -1221,10 +1207,8 @@
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>0.611</t>
-        </is>
+      <c r="AD5" t="n">
+        <v>0.611</v>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
@@ -1236,12 +1220,184 @@
           <t>Jack Link’s Beef Jerky Original</t>
         </is>
       </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>0.611</t>
-        </is>
+      <c r="AG5" t="n">
+        <v>0.611</v>
       </c>
       <c r="AH5" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Hanna Moriel_20251113_214222</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Hanna Moriel</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>21</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-11-13 21:42:22</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.4,
+  "diet": 0.2857142857142857,
+  "salt": 0.8,
+  "fat": 0.4,
+  "natural": 0.2,
+  "convenience": 0.4,
+  "price": 0.2
+}</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0.540</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>0.520</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>0.449</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>0.622</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>0.616</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>0.615</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>0.729</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>0.702</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>0.685</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
         <is>
           <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
         </is>

</xml_diff>

<commit_message>
Actualización automática de grupos experimentales
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -611,7 +611,11 @@
           <t>Salvador Vidal Torres_20251113_180607</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Con SmartScore</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>Salvador Vidal Torres</t>
@@ -767,7 +771,11 @@
           <t>Gerarado Juan_20251113_181055</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Sin SmartScore</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>Gerarado Juan</t>
@@ -923,7 +931,11 @@
           <t>Julieta Hernandez_20251113_204328</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Con SmartScore</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>Julieta Hernandez</t>
@@ -1079,7 +1091,11 @@
           <t>Fernanda Adamaris_20251113_204405</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Sin SmartScore</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>Fernanda Adamaris</t>
@@ -1235,7 +1251,11 @@
           <t>Hanna Moriel_20251113_214222</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Con SmartScore</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>Hanna Moriel</t>
@@ -1272,10 +1292,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>0.540</t>
-        </is>
+      <c r="I6" t="n">
+        <v>0.54</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1287,10 +1305,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>0.520</t>
-        </is>
+      <c r="L6" t="n">
+        <v>0.52</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
@@ -1302,10 +1318,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>0.449</t>
-        </is>
+      <c r="O6" t="n">
+        <v>0.449</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
@@ -1317,10 +1331,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>0.622</t>
-        </is>
+      <c r="R6" t="n">
+        <v>0.622</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
@@ -1332,10 +1344,8 @@
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>0.616</t>
-        </is>
+      <c r="U6" t="n">
+        <v>0.616</v>
       </c>
       <c r="V6" t="inlineStr">
         <is>
@@ -1347,10 +1357,8 @@
           <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
         </is>
       </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>0.615</t>
-        </is>
+      <c r="X6" t="n">
+        <v>0.615</v>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
@@ -1362,10 +1370,8 @@
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>0.729</t>
-        </is>
+      <c r="AA6" t="n">
+        <v>0.729</v>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
@@ -1377,10 +1383,8 @@
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>0.702</t>
-        </is>
+      <c r="AD6" t="n">
+        <v>0.702</v>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
@@ -1392,10 +1396,8 @@
           <t>Jack Link’s Beef Jerky Original</t>
         </is>
       </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>0.685</t>
-        </is>
+      <c r="AG6" t="n">
+        <v>0.6850000000000001</v>
       </c>
       <c r="AH6" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Omar Huerta)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH6"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1405,6 +1405,180 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Omar Huerta_20251119_152531</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Omar Huerta</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>42</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-11-19 15:25:32</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 0.8571428571428571,
+  "salt": 0.6,
+  "fat": 0.4,
+  "natural": 1.0,
+  "convenience": 1.0,
+  "price": 0.8
+}</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0.602</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>0.497</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>0.449</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>0.643</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>0.571</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>0.522</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>0.734</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>0.553</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>0.540</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Alejandra Hidalgo)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1565,6 +1565,180 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Alejandra Hidalgo_20251120_040641</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alejandra Hidalgo</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>21</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-11-20 04:06:42</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 1.0,
+  "salt": 0.8,
+  "fat": 0.8,
+  "natural": 1.0,
+  "convenience": 0.6,
+  "price": 1.0
+}</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0.569</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>0.484</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>0.467</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>0.640</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>0.602</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>0.582</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>0.700</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>0.572</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>0.551</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Maribel Badillo)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AH9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1608,10 +1608,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>0.569</t>
-        </is>
+      <c r="I8" t="n">
+        <v>0.569</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1623,10 +1621,8 @@
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>0.484</t>
-        </is>
+      <c r="L8" t="n">
+        <v>0.484</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
@@ -1638,10 +1634,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>0.467</t>
-        </is>
+      <c r="O8" t="n">
+        <v>0.467</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
@@ -1653,10 +1647,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>0.640</t>
-        </is>
+      <c r="R8" t="n">
+        <v>0.64</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
@@ -1668,10 +1660,8 @@
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>0.602</t>
-        </is>
+      <c r="U8" t="n">
+        <v>0.602</v>
       </c>
       <c r="V8" t="inlineStr">
         <is>
@@ -1683,59 +1673,225 @@
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="X8" t="inlineStr">
+      <c r="X8" t="n">
+        <v>0.582</v>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA8" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.572</v>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG8" t="n">
+        <v>0.551</v>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Maribel Badillo_20251120_154905</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Maribel Badillo</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>21</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-11-20 15:49:06</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 0.14285714285714285,
+  "salt": 0.0,
+  "fat": 1.0,
+  "natural": 0.8,
+  "convenience": 0.0,
+  "price": 0.4
+}</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>0.710</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>0.438</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>0.429</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>0.761</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>0.706</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>0.517</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>0.670</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
         <is>
           <t>0.582</t>
         </is>
       </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
-        </is>
-      </c>
-      <c r="Z8" t="inlineStr">
-        <is>
-          <t>Wild Planet Wild Tuna Pasta Salad</t>
-        </is>
-      </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>0.700</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
-        </is>
-      </c>
-      <c r="AC8" t="inlineStr">
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
         <is>
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="AD8" t="inlineStr">
-        <is>
-          <t>0.572</t>
-        </is>
-      </c>
-      <c r="AE8" t="inlineStr">
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>0.447</t>
+        </is>
+      </c>
+      <c r="AH9" t="inlineStr">
         <is>
           <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
-        </is>
-      </c>
-      <c r="AF8" t="inlineStr">
-        <is>
-          <t>Jack Link’s Beef Jerky Original</t>
-        </is>
-      </c>
-      <c r="AG8" t="inlineStr">
-        <is>
-          <t>0.551</t>
-        </is>
-      </c>
-      <c r="AH8" t="inlineStr">
-        <is>
-          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Ilse Aguirre)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH9"/>
+  <dimension ref="A1:AH10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1764,10 +1764,8 @@
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>0.710</t>
-        </is>
+      <c r="I9" t="n">
+        <v>0.71</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1779,10 +1777,8 @@
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>0.438</t>
-        </is>
+      <c r="L9" t="n">
+        <v>0.438</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
@@ -1794,10 +1790,8 @@
           <t>Nongshim Shin Ramyun</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>0.429</t>
-        </is>
+      <c r="O9" t="n">
+        <v>0.429</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
@@ -1809,10 +1803,8 @@
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>0.761</t>
-        </is>
+      <c r="R9" t="n">
+        <v>0.761</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
@@ -1824,10 +1816,8 @@
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>0.706</t>
-        </is>
+      <c r="U9" t="n">
+        <v>0.706</v>
       </c>
       <c r="V9" t="inlineStr">
         <is>
@@ -1839,10 +1829,8 @@
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>0.517</t>
-        </is>
+      <c r="X9" t="n">
+        <v>0.517</v>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
@@ -1854,10 +1842,8 @@
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>0.670</t>
-        </is>
+      <c r="AA9" t="n">
+        <v>0.67</v>
       </c>
       <c r="AB9" t="inlineStr">
         <is>
@@ -1869,10 +1855,8 @@
           <t>Kitchens of India Variety Pack</t>
         </is>
       </c>
-      <c r="AD9" t="inlineStr">
-        <is>
-          <t>0.582</t>
-        </is>
+      <c r="AD9" t="n">
+        <v>0.582</v>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
@@ -1884,14 +1868,186 @@
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="AG9" t="inlineStr">
-        <is>
-          <t>0.447</t>
-        </is>
+      <c r="AG9" t="n">
+        <v>0.447</v>
       </c>
       <c r="AH9" t="inlineStr">
         <is>
           <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Ilse Aguirre_20251120_155542</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Ilse Aguirre</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>24</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-11-20 15:55:42</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.4,
+  "diet": 0.7142857142857143,
+  "salt": 0.2,
+  "fat": 0.6,
+  "natural": 0.4,
+  "convenience": 0.2,
+  "price": 0.2
+}</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0.533</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>0.422</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0.419</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>0.631</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>0.622</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>0.587</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>0.762</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>0.544</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>0.497</t>
+        </is>
+      </c>
+      <c r="AH10" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Alys)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH10"/>
+  <dimension ref="A1:AH11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2045,6 +2045,180 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Alys_20251120_203615</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alys</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-11-20 20:36:15</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 0.8571428571428571,
+  "salt": 0.4,
+  "fat": 1.0,
+  "natural": 0.8,
+  "convenience": 0.8,
+  "price": 0.8
+}</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.579</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>0.479</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>0.469</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>0.601</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>0.559</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>0.547</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>0.715</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>0.590</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>0.567</t>
+        </is>
+      </c>
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Paula Belén Chairez Rosas)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH11"/>
+  <dimension ref="A1:AH12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2205,6 +2205,180 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Paula Belén Chairez Rosas_20251120_205520</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Paula Belén Chairez Rosas</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>20</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Femenino</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-11-20 20:55:20</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.0,
+  "diet": 0.0,
+  "salt": 0.0,
+  "fat": 0.0,
+  "natural": 0.0,
+  "convenience": 0.0,
+  "price": 0.0
+}</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AG12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="AH12" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Laura Tamariz Valdepeña)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2525,6 +2525,180 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Laura Tamariz Valdepeña_20251120_212917</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Laura Tamariz Valdepeña</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>20</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-11-20 21:29:17</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 0.42857142857142855,
+  "salt": 0.4,
+  "fat": 0.8,
+  "natural": 0.6,
+  "convenience": 1.0,
+  "price": 0.6
+}</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0.589</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>0.520</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0.494</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>0.562</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>0.553</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>0.545</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>0.721</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>0.622</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>0.610</t>
+        </is>
+      </c>
+      <c r="AH14" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Isabel Urdiales Sotres)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH14"/>
+  <dimension ref="A1:AH15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2685,6 +2685,180 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Isabel Urdiales Sotres_20251120_223408</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Isabel Urdiales Sotres</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>20</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-11-20 22:34:08</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.0,
+  "diet": 0.0,
+  "salt": 0.0,
+  "fat": 0.0,
+  "natural": 0.0,
+  "convenience": 0.0,
+  "price": 0.0
+}</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="AH15" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Alyne Corona)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH16"/>
+  <dimension ref="A1:AH17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3005,6 +3005,180 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Alyne Corona_20251128_162805</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alyne Corona</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>21</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-11-28 16:28:05</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.4,
+  "diet": 0.2857142857142857,
+  "salt": 0.2,
+  "fat": 0.2,
+  "natural": 1.0,
+  "convenience": 0.2,
+  "price": 0.2
+}</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0.723</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>0.370</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>0.337</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>0.758</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>0.715</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>0.686</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>0.795</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>0.653</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>0.359</t>
+        </is>
+      </c>
+      <c r="AH17" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Emilio Rugerio)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2365,6 +2365,180 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Emilio Rugerio_20251128_172733</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Emilio Rugerio</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>21</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-11-28 17:27:33</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.6,
+  "diet": 0.2857142857142857,
+  "salt": 0.2,
+  "fat": 0.2,
+  "natural": 0.2,
+  "convenience": 0.2,
+  "price": 0.4
+}</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0.642</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>0.615</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0.562</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>0.601</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>0.580</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>0.517</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>0.621</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>0.507</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>0.487</t>
+        </is>
+      </c>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Alexis Sharon)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2525,6 +2525,180 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Alexis Sharon_20251130_195228</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alexis Sharon</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>28</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-11-30 19:52:28</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.4,
+  "diet": 0.2857142857142857,
+  "salt": 0.6,
+  "fat": 0.2,
+  "natural": 0.4,
+  "convenience": 0.2,
+  "price": 0.6
+}</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0.566</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>0.555</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0.530</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>0.674</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>0.602</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>0.595</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>0.637</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>0.595</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>0.594</t>
+        </is>
+      </c>
+      <c r="AH14" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Elimina participante desde panel de administración
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH14"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2368,7 +2368,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Emilio Rugerio_20251128_172733</t>
+          <t>Alexis Sharon_20251130_195228</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2378,183 +2378,23 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Emilio Rugerio</t>
+          <t>Alexis Sharon</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-11-28 17:27:33</t>
+          <t>2025-11-30 19:52:28</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
-        <is>
-          <t>{
-  "portion": 0.6,
-  "diet": 0.2857142857142857,
-  "salt": 0.2,
-  "fat": 0.2,
-  "natural": 0.2,
-  "convenience": 0.2,
-  "price": 0.4
-}</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Nongshim Neoguri Spicy Seafood</t>
-        </is>
-      </c>
-      <c r="I13" t="n">
-        <v>0.642</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Nissin Chow Mein Teriyaki Beef</t>
-        </is>
-      </c>
-      <c r="L13" t="n">
-        <v>0.615</v>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>Nongshim Shin Ramyun</t>
-        </is>
-      </c>
-      <c r="O13" t="n">
-        <v>0.5620000000000001</v>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
-        </is>
-      </c>
-      <c r="R13" t="n">
-        <v>0.601</v>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>Kraft Macaroni &amp; Cheese Dinner</t>
-        </is>
-      </c>
-      <c r="U13" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
-        </is>
-      </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>Annie’s Shells &amp; White Cheddar</t>
-        </is>
-      </c>
-      <c r="X13" t="n">
-        <v>0.517</v>
-      </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
-        </is>
-      </c>
-      <c r="Z13" t="inlineStr">
-        <is>
-          <t>Wild Planet Wild Tuna Pasta Salad</t>
-        </is>
-      </c>
-      <c r="AA13" t="n">
-        <v>0.621</v>
-      </c>
-      <c r="AB13" t="inlineStr">
-        <is>
-          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
-        </is>
-      </c>
-      <c r="AC13" t="inlineStr">
-        <is>
-          <t>StarKist Chicken Creations (Chicken Salad)</t>
-        </is>
-      </c>
-      <c r="AD13" t="n">
-        <v>0.507</v>
-      </c>
-      <c r="AE13" t="inlineStr">
-        <is>
-          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
-        </is>
-      </c>
-      <c r="AF13" t="inlineStr">
-        <is>
-          <t>Jack Link’s Beef Jerky Original</t>
-        </is>
-      </c>
-      <c r="AG13" t="n">
-        <v>0.487</v>
-      </c>
-      <c r="AH13" t="inlineStr">
-        <is>
-          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Alexis Sharon_20251130_195228</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Con SmartScore</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Alexis Sharon</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>28</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2025-11-30 19:52:28</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
         <is>
           <t>{
   "portion": 0.4,
@@ -2567,119 +2407,119 @@
 }</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>Nongshim Neoguri Spicy Seafood</t>
         </is>
       </c>
-      <c r="I14" t="n">
+      <c r="I13" t="n">
         <v>0.5659999999999999</v>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>Nissin Chow Mein Teriyaki Beef</t>
         </is>
       </c>
-      <c r="L14" t="n">
+      <c r="L13" t="n">
         <v>0.555</v>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>Maruchan Ramen Sabor Pollo</t>
         </is>
       </c>
-      <c r="O14" t="n">
+      <c r="O13" t="n">
         <v>0.53</v>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>Kraft Macaroni &amp; Cheese Dinner</t>
         </is>
       </c>
-      <c r="R14" t="n">
+      <c r="R13" t="n">
         <v>0.674</v>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="S13" t="inlineStr">
         <is>
           <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
         </is>
       </c>
-      <c r="T14" t="inlineStr">
+      <c r="T13" t="inlineStr">
         <is>
           <t>Annie’s Shells &amp; White Cheddar</t>
         </is>
       </c>
-      <c r="U14" t="n">
+      <c r="U13" t="n">
         <v>0.602</v>
       </c>
-      <c r="V14" t="inlineStr">
+      <c r="V13" t="inlineStr">
         <is>
           <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
         </is>
       </c>
-      <c r="W14" t="inlineStr">
+      <c r="W13" t="inlineStr">
         <is>
           <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
         </is>
       </c>
-      <c r="X14" t="n">
+      <c r="X13" t="n">
         <v>0.595</v>
       </c>
-      <c r="Y14" t="inlineStr">
+      <c r="Y13" t="inlineStr">
         <is>
           <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
         </is>
       </c>
-      <c r="Z14" t="inlineStr">
+      <c r="Z13" t="inlineStr">
         <is>
           <t>Wild Planet Wild Tuna Pasta Salad</t>
         </is>
       </c>
-      <c r="AA14" t="n">
+      <c r="AA13" t="n">
         <v>0.637</v>
       </c>
-      <c r="AB14" t="inlineStr">
+      <c r="AB13" t="inlineStr">
         <is>
           <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
         </is>
       </c>
-      <c r="AC14" t="inlineStr">
+      <c r="AC13" t="inlineStr">
         <is>
           <t>StarKist Chicken Creations (Chicken Salad)</t>
         </is>
       </c>
-      <c r="AD14" t="n">
+      <c r="AD13" t="n">
         <v>0.595</v>
       </c>
-      <c r="AE14" t="inlineStr">
+      <c r="AE13" t="inlineStr">
         <is>
           <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
         </is>
       </c>
-      <c r="AF14" t="inlineStr">
+      <c r="AF13" t="inlineStr">
         <is>
           <t>Jack Link’s Beef Jerky Original</t>
         </is>
       </c>
-      <c r="AG14" t="n">
+      <c r="AG13" t="n">
         <v>0.594</v>
       </c>
-      <c r="AH14" t="inlineStr">
+      <c r="AH13" t="inlineStr">
         <is>
           <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
         </is>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Raul Camargo)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2365,6 +2365,180 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Raul Camargo_20251201_165414</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Raul Camargo</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>21</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-12-01 16:54:14</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.6,
+  "diet": 0.2857142857142857,
+  "salt": 0.2,
+  "fat": 0.2,
+  "natural": 0.8,
+  "convenience": 0.2,
+  "price": 0.2
+}</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0.721</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>0.449</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0.418</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>0.746</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>0.670</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>0.641</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>0.754</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>0.597</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>0.363</t>
+        </is>
+      </c>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Muhammad Luqman)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH10"/>
+  <dimension ref="A1:AH11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2045,6 +2045,180 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Muhammad Luqman_20251202_121800</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Muhammad Luqman</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-12-02 12:18:00</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.0,
+  "diet": 0.0,
+  "salt": 0.0,
+  "fat": 0.0,
+  "natural": 0.0,
+  "convenience": 0.0,
+  "price": 0.0
+}</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Harsevak Sandhu Singh)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH12"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2365,6 +2365,180 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Harsevak Sandhu Singh_20251202_122813</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Harsevak Sandhu Singh</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>18</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-12-02 12:28:13</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 0.7142857142857143,
+  "salt": 0.4,
+  "fat": 0.6,
+  "natural": 0.6,
+  "convenience": 1.0,
+  "price": 0.6
+}</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0.582</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>0.507</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0.484</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>0.596</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>0.536</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>0.520</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>0.733</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>0.594</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>0.570</t>
+        </is>
+      </c>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Felis Bramley)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2525,6 +2525,180 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Felis Bramley_20251202_123358</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Felis Bramley</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>18</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-12-02 12:33:58</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.6,
+  "diet": 0.5714285714285714,
+  "salt": 0.2,
+  "fat": 0.2,
+  "natural": 0.4,
+  "convenience": 0.4,
+  "price": 0.0
+}</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0.602</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>0.494</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0.492</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>0.776</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>0.516</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>0.511</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>0.808</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>0.524</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>0.450</t>
+        </is>
+      </c>
+      <c r="AH14" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Arvand Zare)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH14"/>
+  <dimension ref="A1:AH15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2685,6 +2685,180 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Arvand Zare_20251202_124117</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Arvand Zare</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>19</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-12-02 12:41:18</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.6,
+  "diet": 1.0,
+  "salt": 0.8,
+  "fat": 0.6,
+  "natural": 0.8,
+  "convenience": 0.8,
+  "price": 0.4
+}</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0.523</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>0.457</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>0.427</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>0.668</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>0.588</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>0.557</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>0.778</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>0.591</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>0.559</t>
+        </is>
+      </c>
+      <c r="AH15" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Jake Windham)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH15"/>
+  <dimension ref="A1:AH16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2845,6 +2845,180 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Jake Windham_20251202_124710</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Jake Windham</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>20</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-12-02 12:47:10</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 1.0,
+  "salt": 0.8,
+  "fat": 0.8,
+  "natural": 1.0,
+  "convenience": 0.4,
+  "price": 1.0
+}</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>0.571</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>0.483</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>0.459</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>0.662</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>0.605</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>0.602</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>0.690</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>0.557</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>0.535</t>
+        </is>
+      </c>
+      <c r="AH16" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Hannah Minton)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH16"/>
+  <dimension ref="A1:AH17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3005,6 +3005,180 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Hannah Minton_20251202_125046</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Hannah Minton</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>19</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-12-02 12:50:47</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 1.0,
+  "diet": 0.5714285714285714,
+  "salt": 0.0,
+  "fat": 0.0,
+  "natural": 0.2,
+  "convenience": 0.8,
+  "price": 1.0
+}</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0.693</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>0.688</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>0.681</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>0.566</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>0.510</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>0.440</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>0.597</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>0.522</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>0.507</t>
+        </is>
+      </c>
+      <c r="AH17" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Cosmo Sumner)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH17"/>
+  <dimension ref="A1:AH18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3165,6 +3165,180 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Cosmo Sumner_20251202_125519</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Cosmo Sumner</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>18</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-12-02 12:55:19</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 1.0,
+  "diet": 1.0,
+  "salt": 0.4,
+  "fat": 0.6,
+  "natural": 1.0,
+  "convenience": 1.0,
+  "price": 1.0
+}</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0.619</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>0.507</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>0.482</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>0.611</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>0.568</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>0.512</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>0.710</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>0.541</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>0.517</t>
+        </is>
+      </c>
+      <c r="AH18" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Andrew Moody)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH18"/>
+  <dimension ref="A1:AH19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3325,6 +3325,180 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Andrew Moody_20251202_125927</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Andrew Moody</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>18</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-12-02 12:59:27</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.6,
+  "diet": 0.7142857142857143,
+  "salt": 0.2,
+  "fat": 0.8,
+  "natural": 0.2,
+  "convenience": 0.8,
+  "price": 1.0
+}</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0.572</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>0.554</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>0.540</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>0.591</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>0.541</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>0.460</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>0.674</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>0.659</t>
+        </is>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>0.650</t>
+        </is>
+      </c>
+      <c r="AH19" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Harrison Driver)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH19"/>
+  <dimension ref="A1:AH20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3485,6 +3485,180 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Harrison Driver_20251202_130401</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Harrison Driver</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>18</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-12-02 13:04:01</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 1.0,
+  "diet": 1.0,
+  "salt": 0.2,
+  "fat": 0.2,
+  "natural": 0.8,
+  "convenience": 1.0,
+  "price": 0.8
+}</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0.646</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>0.543</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>0.535</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>0.662</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>0.507</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>0.456</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>0.720</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>0.498</t>
+        </is>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>Kitchens of India Variety Pack</t>
+        </is>
+      </c>
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t>0.472</t>
+        </is>
+      </c>
+      <c r="AH20" t="inlineStr">
+        <is>
+          <t>Sabor auténtico, variedad, vegetariano, necesita arroz o pan, buena calidad</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Edward Hira)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH21"/>
+  <dimension ref="A1:AH22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3805,6 +3805,180 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Edward Hira_20251202_131403</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Edward Hira</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>18</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-12-02 13:14:04</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 1.0,
+  "salt": 0.6,
+  "fat": 0.8,
+  "natural": 0.8,
+  "convenience": 1.0,
+  "price": 0.8
+}</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>0.561</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>0.486</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>0.473</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>0.595</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>0.573</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>0.524</t>
+        </is>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z22" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>0.730</t>
+        </is>
+      </c>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD22" t="inlineStr">
+        <is>
+          <t>0.600</t>
+        </is>
+      </c>
+      <c r="AE22" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG22" t="inlineStr">
+        <is>
+          <t>0.573</t>
+        </is>
+      </c>
+      <c r="AH22" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (Robbie Sweetin)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH22"/>
+  <dimension ref="A1:AH23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3965,6 +3965,180 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Robbie Sweetin_20251202_131942</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Robbie Sweetin</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>18</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-12-02 13:19:42</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.6,
+  "diet": 0.7142857142857143,
+  "salt": 0.4,
+  "fat": 0.8,
+  "natural": 0.6,
+  "convenience": 0.4,
+  "price": 0.6
+}</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>0.562</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>0.468</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>0.465</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>0.636</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>0.581</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>0.569</t>
+        </is>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>0.706</t>
+        </is>
+      </c>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD23" t="inlineStr">
+        <is>
+          <t>0.582</t>
+        </is>
+      </c>
+      <c r="AE23" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG23" t="inlineStr">
+        <is>
+          <t>0.556</t>
+        </is>
+      </c>
+      <c r="AH23" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (dima roman tarabzouni)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH23"/>
+  <dimension ref="A1:AH24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4125,6 +4125,180 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>dima roman tarabzouni_20251202_133740</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>dima roman tarabzouni</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>20</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-12-02 13:37:40</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.8,
+  "diet": 1.0,
+  "salt": 0.4,
+  "fat": 0.6,
+  "natural": 0.4,
+  "convenience": 0.0,
+  "price": 1.0
+}</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>0.576</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>0.558</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Nongshim Shin Ramyun</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>0.498</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Sabor intenso, picante, umami, fideos gruesos, muy alto en sodio</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>0.647</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>0.570</t>
+        </is>
+      </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>0.567</t>
+        </is>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="Z24" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>0.610</t>
+        </is>
+      </c>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AD24" t="inlineStr">
+        <is>
+          <t>0.532</t>
+        </is>
+      </c>
+      <c r="AE24" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AG24" t="inlineStr">
+        <is>
+          <t>0.501</t>
+        </is>
+      </c>
+      <c r="AH24" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (remas ali almadani)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH24"/>
+  <dimension ref="A1:AH25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4285,6 +4285,180 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>remas ali almadani_20251202_134128</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>remas ali almadani</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>19</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-12-02 13:41:28</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.2,
+  "diet": 0.2857142857142857,
+  "salt": 0.6,
+  "fat": 0.6,
+  "natural": 0.8,
+  "convenience": 0.4,
+  "price": 1.0
+}</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>0.578</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>0.566</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>0.455</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>0.712</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>Annie’s Shells &amp; White Cheddar</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>0.625</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>Queso blanco real, sin colorantes, sabor casero, menos salado, buena para niños</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>0.567</t>
+        </is>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="Z25" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>0.657</t>
+        </is>
+      </c>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+      <c r="AC25" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AD25" t="inlineStr">
+        <is>
+          <t>0.656</t>
+        </is>
+      </c>
+      <c r="AE25" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+      <c r="AF25" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AG25" t="inlineStr">
+        <is>
+          <t>0.644</t>
+        </is>
+      </c>
+      <c r="AH25" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización SmartScore desde Streamlit (xiaoyi)
</commit_message>
<xml_diff>
--- a/Resultados_SmartScore.xlsx
+++ b/Resultados_SmartScore.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH27"/>
+  <dimension ref="A1:AH28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4765,6 +4765,180 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>xiaoyi_20251202_134614</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>xiaoyi</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>26</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-12-02 13:46:14</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>{
+  "portion": 0.4,
+  "diet": 0.7142857142857143,
+  "salt": 0.2,
+  "fat": 0.8,
+  "natural": 0.2,
+  "convenience": 1.0,
+  "price": 1.0
+}</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Maruchan Ramen Sabor Pollo</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>0.591</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Sabor clásico, económico, alto en sodio, no saludable, nostálgico</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Nongshim Neoguri Spicy Seafood</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>0.532</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Sabor a marisco, umami, picante equilibrado, buena textura, algo salado</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Nissin Chow Mein Teriyaki Beef</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>0.518</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Fácil de preparar, porción generosa, salsa suave, necesita mejoras, alto en grasa</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>Velveeta Original Shells &amp; Cheese (microwave cups)</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>0.607</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>Muy cremoso, porción individual, rápido, salado, ideal para niños</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>Kraft Macaroni &amp; Cheese Dinner</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>0.520</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>Sabor nostálgico, clásico americano, fácil, no muy nutritivo, barato</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>Amy’s Macaroni &amp; Cheese (frozen)</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>0.443</t>
+        </is>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>Queso real, textura casera, sin conservadores, alto en grasa, algo caro</t>
+        </is>
+      </c>
+      <c r="Z28" t="inlineStr">
+        <is>
+          <t>StarKist Chicken Creations (Chicken Salad)</t>
+        </is>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>0.718</t>
+        </is>
+      </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>Portátil, saludable, fácil, buena textura, sabor suave</t>
+        </is>
+      </c>
+      <c r="AC28" t="inlineStr">
+        <is>
+          <t>Jack Link’s Beef Jerky Original</t>
+        </is>
+      </c>
+      <c r="AD28" t="inlineStr">
+        <is>
+          <t>0.705</t>
+        </is>
+      </c>
+      <c r="AE28" t="inlineStr">
+        <is>
+          <t>Ahumado, sabroso, alto en proteína, snack ideal, porción pequeña</t>
+        </is>
+      </c>
+      <c r="AF28" t="inlineStr">
+        <is>
+          <t>Wild Planet Wild Tuna Pasta Salad</t>
+        </is>
+      </c>
+      <c r="AG28" t="inlineStr">
+        <is>
+          <t>0.673</t>
+        </is>
+      </c>
+      <c r="AH28" t="inlineStr">
+        <is>
+          <t>Sabor fresco, buena proteína, saludable, porción algo pequeña</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>